<commit_message>
Update Alpha Test Plan - USB BASIC v1.3.xlsx
</commit_message>
<xml_diff>
--- a/docs/Alpha Test Plan - USB BASIC v1.3.xlsx
+++ b/docs/Alpha Test Plan - USB BASIC v1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Peripherals\Expanders\Aquarius MX\Aquarius-MX\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED4DB5D-F00D-4094-9D16-8655DE6956EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEF51A0-F463-40D2-9A4D-8CA6AACD886F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E4602F1-086A-45F3-8A9B-97B686BB3C0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
   <si>
     <t>Alpha Test Plan</t>
   </si>
@@ -189,12 +189,6 @@
   </si>
   <si>
     <t>System should display a brief listing of the contents of the USB folder within the AquaLite program folder, followed by Ok beneath. Note that the contents can vary from system to system.</t>
-  </si>
-  <si>
-    <t>E-1.1.4.1</t>
-  </si>
-  <si>
-    <t>E-1.1.4.2</t>
   </si>
   <si>
     <t>Test DIR</t>
@@ -425,6 +419,246 @@
   </si>
   <si>
     <t>DO NOT CONTINUE IF ANY TESTS IN THIS SECTION DID NOT PASS! CONTACT THE TESTING COORDINATOR.</t>
+  </si>
+  <si>
+    <t>E-1.1.3.1</t>
+  </si>
+  <si>
+    <t>E-1.1.3.2</t>
+  </si>
+  <si>
+    <t>E-1.1.4</t>
+  </si>
+  <si>
+    <t>Test CLS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the USB BASIC command screen type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>CLS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  and hit RETURN</t>
+    </r>
+  </si>
+  <si>
+    <t>E-1.1.5.1</t>
+  </si>
+  <si>
+    <t>E-1.1.5.2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the USB BASIC command screen type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>CLS 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  and hit RETURN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System should clear the screen and show Ok in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>black</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> letters on a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cyan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> background.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System should clear the screen and show Ok in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>black</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> letters on a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>grey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> background.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the USB BASIC command screen type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>CLS $7D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  and hit RETURN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System should clear the screen and show Ok in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>white</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> letters on a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dark green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> background.</t>
+    </r>
+  </si>
+  <si>
+    <t>E-1.1.5.3</t>
+  </si>
+  <si>
+    <t>E-1.1.5.4</t>
   </si>
 </sst>
 </file>
@@ -825,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -841,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -862,18 +1096,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -898,50 +1129,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1305,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7D3E11-A3ED-4CC5-A1AF-BE2B1210CD44}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,20 +1552,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1390,12 +1621,12 @@
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1411,10 +1642,10 @@
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="23"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1430,10 +1661,10 @@
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="23"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1449,10 +1680,10 @@
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="23"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1468,10 +1699,10 @@
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="23"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -1487,39 +1718,39 @@
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="23"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="27" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="29"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
+      <c r="A16" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
@@ -1538,7 +1769,7 @@
       <c r="B18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="29" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -1573,22 +1804,22 @@
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>39</v>
@@ -1596,37 +1827,37 @@
       <c r="F20" s="9"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="38"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>39</v>
@@ -1634,37 +1865,37 @@
       <c r="F22" s="9"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="23"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>39</v>
@@ -1672,39 +1903,39 @@
       <c r="F24" s="9"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="23"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="26" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="23"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>50</v>
@@ -1712,176 +1943,258 @@
       <c r="F26" s="9"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="23"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>51</v>
+      <c r="A27" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="42" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="23"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>52</v>
+      <c r="A28" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="23"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>37</v>
+      <c r="A29" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="23"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="41" t="s">
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B38" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="44"/>
-    </row>
-    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="35"/>
+    </row>
+    <row r="39" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -2563,14 +2876,95 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A39:I39"/>
     <mergeCell ref="C20:C25"/>
     <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C30:C33"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test plan updates, etc
</commit_message>
<xml_diff>
--- a/docs/Alpha Test Plan - USB BASIC v1.3.xlsx
+++ b/docs/Alpha Test Plan - USB BASIC v1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Peripherals\Expanders\Aquarius MX\Aquarius-MX\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01639EF2-569F-411E-9D36-7079239474D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375A2E4B-D500-4861-9853-2517FC05B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E4602F1-086A-45F3-8A9B-97B686BB3C0F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="235">
   <si>
     <t>Alpha Test Plan</t>
   </si>
@@ -1562,12 +1562,6 @@
     <t>Test POKE range</t>
   </si>
   <si>
-    <t>E-1.1.2.1</t>
-  </si>
-  <si>
-    <t>E-1.1.2.2</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">From the USB BASIC command screen type the code below and hit RETURN:
 </t>
@@ -1599,6 +1593,9 @@
       </rPr>
       <t>POKE $3291,97,STEP 40,97,STEP 40,97</t>
     </r>
+  </si>
+  <si>
+    <t>Test POKE auto-increment</t>
   </si>
   <si>
     <r>
@@ -1613,7 +1610,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>aaa</t>
+      <t>aaaaaaaaa</t>
     </r>
     <r>
       <rPr>
@@ -1623,11 +1620,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (three letter a's) in a downward right diagonal towards the middle bottom of the screen.</t>
-    </r>
-  </si>
-  <si>
-    <t>Test POKE auto-increment</t>
+      <t xml:space="preserve"> (nine letter a's) in a row towards the middle bottom of the screen.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1642,7 +1636,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>aaaaaaaaa</t>
+      <t>abcd</t>
     </r>
     <r>
       <rPr>
@@ -1652,12 +1646,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (nine letter a's) in a row towards the middle bottom of the screen.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The screen should print </t>
+      <t xml:space="preserve"> in a row towards the middle bottom of the screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Legacy Commands</t>
+  </si>
+  <si>
+    <t>New Commands</t>
+  </si>
+  <si>
+    <t>Test COPY</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System should boot into "BASIC Press RETURN key to start" flashing screen. Menubar should say </t>
     </r>
     <r>
       <rPr>
@@ -1668,7 +1674,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>abcd</t>
+      <t>AquaLite v1.36</t>
     </r>
     <r>
       <rPr>
@@ -1678,24 +1684,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> in a row towards the middle bottom of the screen.</t>
-    </r>
-  </si>
-  <si>
-    <t>Setup</t>
-  </si>
-  <si>
-    <t>Legacy Commands</t>
-  </si>
-  <si>
-    <t>New Commands</t>
-  </si>
-  <si>
-    <t>Test COPY</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">System should boot into "BASIC Press RETURN key to start" flashing screen. Menubar should say </t>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The screen should print </t>
     </r>
     <r>
       <rPr>
@@ -1706,7 +1700,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AquaLite v1.36</t>
+      <t>aaa</t>
     </r>
     <r>
       <rPr>
@@ -1716,7 +1710,90 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.</t>
+      <t xml:space="preserve"> (three letter a's) in a downward line at the middle bottom of the screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Test POKE strings</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the USB BASIC command screen type the code below and hit RETURN:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>POKE $3291,"Hubba",STEP 40,"Bubba"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The screen should print the words </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hubba Bubba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> stacked on top of each other at the middle bottom of the screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>E-1.2.1.2</t>
+  </si>
+  <si>
+    <t>E-1.2.2.1</t>
+  </si>
+  <si>
+    <t>E-1.2.2.2</t>
+  </si>
+  <si>
+    <t>E-1.2.3.1</t>
+  </si>
+  <si>
+    <t>E-1.2.3.2</t>
+  </si>
+  <si>
+    <t>E-1.2.4.1</t>
+  </si>
+  <si>
+    <t>E-1.2.4.2</t>
+  </si>
+  <si>
+    <t>The text at the top of the screen ("Copyright © 1982 by Microsoft, Inc S2" &amp; "USB BASIC v1.3" should be duplicated in the middle of the screen, with the Ok beneath the COPY command near the top.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the USB BASIC command screen type the code below and hit RETURN:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>COPY $3000,$3000+440,120</t>
     </r>
   </si>
 </sst>
@@ -2642,8 +2719,8 @@
   </sheetPr>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A100" sqref="A99:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,7 +2763,7 @@
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B7" s="35"/>
     </row>
@@ -2767,7 +2844,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
@@ -2875,7 +2952,7 @@
     </row>
     <row r="18" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="35" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B18" s="35"/>
       <c r="D18" s="5"/>
@@ -4193,7 +4270,7 @@
     </row>
     <row r="86" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="35" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B86" s="35"/>
       <c r="D86" s="5"/>
@@ -4257,7 +4334,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>38</v>
@@ -4272,7 +4349,7 @@
     </row>
     <row r="90" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="29" t="s">
-        <v>40</v>
+        <v>226</v>
       </c>
       <c r="B90" s="30" t="s">
         <v>13</v>
@@ -4282,7 +4359,7 @@
         <v>208</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
@@ -4291,7 +4368,7 @@
     </row>
     <row r="91" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="B91" s="30" t="s">
         <v>13</v>
@@ -4312,17 +4389,17 @@
     </row>
     <row r="92" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="29" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="B92" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="43"/>
       <c r="D92" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F92" s="8"/>
       <c r="G92" s="9"/>
@@ -4331,13 +4408,13 @@
     </row>
     <row r="93" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
-        <v>60</v>
+        <v>229</v>
       </c>
       <c r="B93" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>64</v>
@@ -4352,97 +4429,97 @@
     </row>
     <row r="94" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="29" t="s">
-        <v>61</v>
+        <v>230</v>
       </c>
       <c r="B94" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="43"/>
       <c r="D94" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
       <c r="I94" s="18"/>
     </row>
-    <row r="95" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
-        <v>201</v>
+        <v>231</v>
       </c>
       <c r="B95" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="36" t="s">
         <v>223</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E95" s="21" t="s">
-        <v>24</v>
+        <v>64</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="F95" s="8"/>
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
       <c r="I95" s="18"/>
     </row>
-    <row r="96" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="29" t="s">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="B96" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C96" s="8"/>
+      <c r="C96" s="38"/>
       <c r="D96" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>198</v>
+        <v>224</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>225</v>
       </c>
       <c r="F96" s="8"/>
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
       <c r="I96" s="18"/>
     </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="29" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="B97" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C97" s="8"/>
+      <c r="C97" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D97" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>200</v>
+        <v>38</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="F97" s="8"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
       <c r="I97" s="18"/>
     </row>
-    <row r="98" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="29" t="s">
-        <v>201</v>
+        <v>66</v>
       </c>
       <c r="B98" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C98" s="8" t="s">
-        <v>196</v>
-      </c>
+      <c r="C98" s="38"/>
       <c r="D98" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>78</v>
+        <v>234</v>
+      </c>
+      <c r="E98" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="F98" s="8"/>
       <c r="G98" s="9"/>
@@ -4451,12 +4528,14 @@
     </row>
     <row r="99" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
-        <v>202</v>
+        <v>87</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C99" s="8"/>
+      <c r="C99" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D99" s="7" t="s">
         <v>112</v>
       </c>
@@ -4470,12 +4549,14 @@
     </row>
     <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>203</v>
+        <v>88</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C100" s="8"/>
+      <c r="C100" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D100" s="7" t="s">
         <v>199</v>
       </c>
@@ -4494,8 +4575,8 @@
       <c r="B101" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>196</v>
+      <c r="C101" s="46" t="s">
+        <v>223</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>197</v>
@@ -4515,7 +4596,9 @@
       <c r="B102" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C102" s="8"/>
+      <c r="C102" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D102" s="7" t="s">
         <v>112</v>
       </c>
@@ -4534,7 +4617,9 @@
       <c r="B103" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C103" s="8"/>
+      <c r="C103" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D103" s="7" t="s">
         <v>199</v>
       </c>
@@ -4553,8 +4638,8 @@
       <c r="B104" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>196</v>
+      <c r="C104" s="46" t="s">
+        <v>223</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>197</v>
@@ -4574,7 +4659,9 @@
       <c r="B105" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C105" s="8"/>
+      <c r="C105" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D105" s="7" t="s">
         <v>112</v>
       </c>
@@ -4593,7 +4680,9 @@
       <c r="B106" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C106" s="8"/>
+      <c r="C106" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D106" s="7" t="s">
         <v>199</v>
       </c>
@@ -4612,8 +4701,8 @@
       <c r="B107" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>196</v>
+      <c r="C107" s="46" t="s">
+        <v>223</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>197</v>
@@ -4633,7 +4722,9 @@
       <c r="B108" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C108" s="8"/>
+      <c r="C108" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D108" s="7" t="s">
         <v>112</v>
       </c>
@@ -4652,7 +4743,9 @@
       <c r="B109" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C109" s="8"/>
+      <c r="C109" s="46" t="s">
+        <v>223</v>
+      </c>
       <c r="D109" s="7" t="s">
         <v>199</v>
       </c>
@@ -4777,7 +4870,7 @@
       <c r="I119" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:I16"/>
@@ -4805,6 +4898,8 @@
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="C72:C79"/>
     <mergeCell ref="C80:C83"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>